<commit_message>
Modify plots with bigger fonts and svg.
</commit_message>
<xml_diff>
--- a/statistics/Book1.xlsx
+++ b/statistics/Book1.xlsx
@@ -8,104 +8,126 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galina/bachelor_thesis/statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1D87BC-0AE2-7C40-BC07-A89535B46D41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AA00F2-CCE7-744D-B9CC-4F6D82970BA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="2" xr2:uid="{855680A4-7707-4643-B0AE-4203C6A3D4C2}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="4" xr2:uid="{855680A4-7707-4643-B0AE-4203C6A3D4C2}"/>
   </bookViews>
   <sheets>
     <sheet name="dry_run_avg" sheetId="1" r:id="rId1"/>
     <sheet name="dry_run_perc" sheetId="2" r:id="rId2"/>
     <sheet name="sim_avg" sheetId="5" r:id="rId3"/>
     <sheet name="sim_perc" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">sim_avg!$B$2:$B$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">sim_avg!$E$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">sim_perc!$A$2</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">sim_perc!$A$3</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">sim_perc!$A$4</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">sim_perc!$A$5</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">sim_perc!$A$6</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">sim_perc!$A$7</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">sim_perc!$B$1:$K$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">sim_perc!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">sim_perc!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">sim_avg!$E$2:$E$7</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">sim_perc!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">sim_perc!$B$6:$K$6</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">sim_perc!$B$7:$K$7</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">sim_perc!$A$2</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">sim_perc!$A$3</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">sim_perc!$A$4</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">sim_perc!$A$5</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">sim_perc!$A$6</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">sim_perc!$A$7</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">sim_perc!$B$1:$K$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">sim_avg!$P$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">sim_perc!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">sim_perc!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">sim_perc!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">sim_perc!$B$6:$K$6</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">sim_perc!$B$7:$K$7</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">sim_perc!$A$2</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">sim_perc!$A$3</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">sim_perc!$A$4</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">sim_perc!$A$5</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">sim_avg!$P$2:$P$7</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">sim_perc!$A$6</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">sim_perc!$A$7</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">sim_perc!$B$1:$K$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">sim_perc!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">sim_perc!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">sim_perc!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">sim_perc!$B$6:$K$6</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">sim_perc!$B$7:$K$7</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">sim_perc!$B$10:$K$10</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">sim_perc!$B$1:$K$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">sim_perc!$B$9:$K$9</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">sim_perc!$A$2</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">sim_perc!$A$3</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">sim_perc!$A$4</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">sim_perc!$A$5</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">sim_perc!$A$6</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">sim_perc!$A$7</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">sim_perc!$B$1:$K$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">sim_perc!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">sim_perc!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">sim_perc!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">sim_perc!$B$6:$K$6</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">sim_perc!$B$7:$K$7</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">sim_perc!$A$2</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">sim_perc!$A$3</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">sim_perc!$A$4</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">sim_perc!$A$5</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">sim_perc!$A$6</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">sim_perc!$A$7</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">sim_perc!$B$1:$K$1</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">sim_perc!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">sim_perc!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">sim_perc!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">sim_perc!$B$6:$K$6</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">sim_perc!$B$7:$K$7</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">sim_perc!$B$10:$K$10</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">sim_perc!$B$1:$K$1</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">sim_perc!$B$9:$K$9</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">sim_perc!$B$10:$K$10</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">dry_run_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">dry_run_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">dry_run_perc!$C$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.100" hidden="1">sim_perc!$A$7</definedName>
+    <definedName name="_xlchart.v1.101" hidden="1">sim_perc!$B$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.102" hidden="1">sim_perc!$B$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.103" hidden="1">sim_perc!$B$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.104" hidden="1">sim_perc!$B$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.105" hidden="1">sim_perc!$B$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.106" hidden="1">sim_perc!$B$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.107" hidden="1">sim_perc!$B$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">dry_run_perc!$C$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">dry_run_perc!$C$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">dry_run_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">dry_run_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">dry_run_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">dry_run_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">dry_run_perc!$A$6</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">dry_run_perc!$A$7</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">dry_run_perc!$C$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">dry_run_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">dry_run_perc!$C$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">dry_run_perc!$C$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">dry_run_perc!$C$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">dry_run_perc!$C$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">dry_run_perc!$C$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">dry_run_perc!$C$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">dry_run_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">dry_run_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">dry_run_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">dry_run_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">dry_run_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">dry_run_perc!$A$6</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">dry_run_perc!$A$7</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">dry_run_perc!$C$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">dry_run_perc!$C$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">dry_run_perc!$C$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">dry_run_perc!$C$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">dry_run_perc!$C$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">dry_run_perc!$C$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">dry_run_perc!$C$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">dry_run_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">dry_run_perc!$A$6</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">dry_run_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">dry_run_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">dry_run_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">dry_run_perc!$A$6</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">dry_run_perc!$A$7</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">dry_run_perc!$C$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">dry_run_perc!$C$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">dry_run_perc!$C$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">dry_run_perc!$C$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">dry_run_perc!$C$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">dry_run_perc!$A$7</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">dry_run_perc!$C$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">dry_run_perc!$C$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">dry_run_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">dry_run_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">dry_run_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">dry_run_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">dry_run_perc!$A$6</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">dry_run_perc!$A$7</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">dry_run_perc!$C$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">dry_run_perc!$C$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">dry_run_perc!$C$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">dry_run_perc!$C$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">dry_run_perc!$C$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">dry_run_perc!$C$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">dry_run_perc!$C$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">dry_run_perc!$C$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">dry_run_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">dry_run_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">dry_run_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">dry_run_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">dry_run_perc!$A$6</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">dry_run_perc!$C$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">dry_run_perc!$A$7</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">dry_run_perc!$C$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">dry_run_perc!$C$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">dry_run_perc!$C$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">dry_run_perc!$C$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">dry_run_perc!$C$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">dry_run_perc!$C$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">dry_run_perc!$C$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">sim_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">sim_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">dry_run_perc!$C$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">sim_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">sim_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">sim_perc!$A$6</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">sim_perc!$A$7</definedName>
     <definedName name="_xlchart.v1.84" hidden="1">sim_perc!$B$1:$K$1</definedName>
     <definedName name="_xlchart.v1.85" hidden="1">sim_perc!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">sim_perc!$B$9:$K$9</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">sim_avg!$B$2:$B$7</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">sim_avg!$E$1</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">sim_avg!$E$2:$E$7</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">sim_avg!$P$1</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">sim_avg!$P$2:$P$7</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">sim_perc!$B$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">sim_perc!$B$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">sim_perc!$B$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">sim_perc!$B$6:$K$6</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">dry_run_perc!$C$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">sim_perc!$B$7:$K$7</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">sim_perc!$B$10:$K$10</definedName>
+    <definedName name="_xlchart.v1.92" hidden="1">sim_perc!$B$1:$K$1</definedName>
+    <definedName name="_xlchart.v1.93" hidden="1">sim_perc!$B$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.94" hidden="1">sim_perc!$B$9:$K$9</definedName>
+    <definedName name="_xlchart.v1.95" hidden="1">sim_perc!$A$2</definedName>
+    <definedName name="_xlchart.v1.96" hidden="1">sim_perc!$A$3</definedName>
+    <definedName name="_xlchart.v1.97" hidden="1">sim_perc!$A$4</definedName>
+    <definedName name="_xlchart.v1.98" hidden="1">sim_perc!$A$5</definedName>
+    <definedName name="_xlchart.v1.99" hidden="1">sim_perc!$A$6</definedName>
     <definedName name="distribution_1563839199.0174332" localSheetId="1">dry_run_perc!$A$1:$K$7</definedName>
     <definedName name="distribution_1563839199.0174332_1" localSheetId="3">sim_perc!$A$1:$K$7</definedName>
     <definedName name="distribution_1563839199.0174332_2" localSheetId="3">sim_perc!$A$9:$K$15</definedName>
@@ -216,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="61">
   <si>
     <t>Method</t>
   </si>
@@ -303,6 +325,102 @@
   </si>
   <si>
     <t>3.02</t>
+  </si>
+  <si>
+    <t>GET /reviews/10: "ConnectionError(ProtocolError('Connection aborted.', ConnectionResetError(54, 'Connection reset by peer')))"</t>
+  </si>
+  <si>
+    <t>GET /reviews/restaurant/10: "ConnectionError(ProtocolError('Connection aborted.', ConnectionResetError(54, 'Connection reset by peer')))"</t>
+  </si>
+  <si>
+    <t>GET /reviews/: "ConnectionError(ProtocolError('Connection aborted.', ConnectionResetError(54, 'Connection reset by peer')))"</t>
+  </si>
+  <si>
+    <t>GET /reviews/user/10: "ConnectionError(ProtocolError('Connection aborted.', ConnectionResetError(54, 'Connection reset by peer')))"</t>
+  </si>
+  <si>
+    <t>GET /reviews/: 'ConnectionError(MaxRetryError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Max retries exceeded with url: /reviews/ (Caused by NewConnectionError(\'&lt;urllib3.connection.HTTPConnection object at 0x10ab02320&gt;: Failed to establish a new connection: [Errno 60] Operation timed out\'))"))'</t>
+  </si>
+  <si>
+    <t>GET /reviews/restaurant/10: 'ConnectionError(MaxRetryError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Max retries exceeded with url: /reviews/restaurant/10 (Caused by NewConnectionError(\'&lt;urllib3.connection.HTTPConnection object at 0x10ab47ef0&gt;: Failed to establish a new connection: [Errno 60] Operation timed out\'))"))'</t>
+  </si>
+  <si>
+    <t>GET /reviews/user/10: 'ConnectionError(MaxRetryError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Max retries exceeded with url: /reviews/user/10 (Caused by NewConnectionError(\'&lt;urllib3.connection.HTTPConnection object at 0x10ac2ffd0&gt;: Failed to establish a new connection: [Errno 60] Operation timed out\'))"))'</t>
+  </si>
+  <si>
+    <t>GET /reviews/10: 'ConnectionError(MaxRetryError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Max retries exceeded with url: /reviews/10 (Caused by NewConnectionError(\'&lt;urllib3.connection.HTTPConnection object at 0x10adab828&gt;: Failed to establish a new connection: [Errno 60] Operation timed out\'))"))'</t>
+  </si>
+  <si>
+    <t>GET /reviews/user/10: 'ReadTimeout(ReadTimeoutError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Read timed out. (read timeout=None)"))'</t>
+  </si>
+  <si>
+    <t>GET /reviews/: 'ReadTimeout(ReadTimeoutError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Read timed out. (read timeout=None)"))'</t>
+  </si>
+  <si>
+    <t>GET /reviews/10: 'ReadTimeout(ReadTimeoutError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Read timed out. (read timeout=None)"))'</t>
+  </si>
+  <si>
+    <t>GET /reviews/restaurant/10: 'ReadTimeout(ReadTimeoutError("HTTPConnectionPool(host=\'34.65.220.187\', port=8080): Read timed out. (read timeout=None)"))'</t>
+  </si>
+  <si>
+    <t>Number of occurrences</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>ConnectionResetError(54, 'Connection reset by peer')</t>
+  </si>
+  <si>
+    <t>Failed to establish a new connection: [Errno 60] Operation timed out\'</t>
+  </si>
+  <si>
+    <t>Read timed out.</t>
+  </si>
+  <si>
+    <t>GET /reviews/10: "HTTPError('502 Server Error: Bad Gateway for url: http://34.65.88.84/reviews/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/: "HTTPError('502 Server Error: Bad Gateway for url: http://34.65.88.84/reviews/')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/user/10: "HTTPError('502 Server Error: Bad Gateway for url: http://34.65.88.84/reviews/user/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/restaurant/10: "HTTPError('502 Server Error: Bad Gateway for url: http://34.65.88.84/reviews/restaurant/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/restaurant/10: "HTTPError('503 Server Error: Service Unavailable for url: http://34.65.88.84/reviews/restaurant/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/: "HTTPError('503 Server Error: Service Unavailable for url: http://34.65.88.84/reviews/')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/10: "HTTPError('503 Server Error: Service Unavailable for url: http://34.65.88.84/reviews/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/user/10: "HTTPError('503 Server Error: Service Unavailable for url: http://34.65.88.84/reviews/user/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/10: "HTTPError('500 Server Error: Internal Server Error for url: http://34.65.88.84/reviews/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/user/10: "HTTPError('500 Server Error: Internal Server Error for url: http://34.65.88.84/reviews/user/10')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/: "HTTPError('500 Server Error: Internal Server Error for url: http://34.65.88.84/reviews/')"</t>
+  </si>
+  <si>
+    <t>GET /reviews/restaurant/10: "HTTPError('500 Server Error: Internal Server Error for url: http://34.65.88.84/reviews/restaurant/10')"</t>
+  </si>
+  <si>
+    <t>500 Server Error: Internal Server Error</t>
+  </si>
+  <si>
+    <t>503 Server Error: Service Unavailable</t>
+  </si>
+  <si>
+    <t>502 Server Error: Bad Gateway</t>
   </si>
 </sst>
 </file>
@@ -9220,7 +9338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C91E46C-3509-4C4F-BDDF-654864F458C9}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection sqref="A1:J7"/>
     </sheetView>
   </sheetViews>
@@ -9472,7 +9590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A874471-7325-3B45-B7AE-F0E1B9D088D0}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection sqref="A1:K7"/>
     </sheetView>
   </sheetViews>
@@ -9739,7 +9857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157F7ECD-2621-1C49-A24F-A91FF7B22AFB}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -10211,8 +10329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD4E4507-FE8C-604D-838F-D4C0A43D8CF8}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10717,4 +10835,276 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488146EA-9490-5A4F-B0DB-AF3A8DE1D161}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1185</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1609</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1608</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1626</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1666</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>254</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>272</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>248</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>264</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f>SUM(A3:A6)</f>
+        <v>4636</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f>SUM(A7:A10)</f>
+        <v>6509</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f>SUM(A11:A14)</f>
+        <v>1038</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>6359</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6188</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6266</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6354</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f>SUM(A22:A25)</f>
+        <v>25167</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f>SUM(A26:A29)</f>
+        <v>309</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f>SUM(A30:A33)</f>
+        <v>73</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>